<commit_message>
add script for constructing UCPR mortality tables.
</commit_message>
<xml_diff>
--- a/Data/RP2014/research-2014-rp-mort-tab-rates-exposure.xlsx
+++ b/Data/RP2014/research-2014-rp-mort-tab-rates-exposure.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\PenSim-Projects\Model_Main\Data\RP2014\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="19410" windowHeight="9855"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="24900"/>
   </bookViews>
   <sheets>
     <sheet name="Total Dataset" sheetId="2" r:id="rId1"/>
@@ -14,7 +19,7 @@
     <sheet name="Top Quartile" sheetId="6" r:id="rId5"/>
     <sheet name="Juvenile" sheetId="1" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -96,7 +101,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
@@ -395,6 +400,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -442,7 +450,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -477,7 +485,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4833,7 +4841,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H107"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>